<commit_message>
Works in progress - current messy progress, will refactor and organize soon
</commit_message>
<xml_diff>
--- a/documentation/working_schedule.xlsx
+++ b/documentation/working_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebrarsudedogan/PycharmProjects/Mining-Retail-Behavior-in-Istanbul-Malls-Using-Consumer-Sentiment-Indices/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144311C5-884A-C245-8EF6-BDF747F073DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F99A3-2690-E44D-8CD1-6D083A24CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14280" xr2:uid="{900F4403-C22E-0342-A1F2-D386E10D2AC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
   <si>
     <t>Veri Toplama</t>
   </si>
@@ -551,7 +551,7 @@
   <dimension ref="B3:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -665,8 +665,12 @@
         <v>13</v>
       </c>
       <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="S4" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="T4" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="U4" s="5"/>
       <c r="V4" s="5"/>
       <c r="W4" s="5"/>
@@ -730,7 +734,9 @@
       </c>
       <c r="Q6" s="4"/>
       <c r="R6" s="4"/>
-      <c r="S6" s="4"/>
+      <c r="S6" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="T6" s="4"/>
       <c r="U6" s="4"/>
       <c r="V6" s="4"/>
@@ -796,7 +802,9 @@
       </c>
       <c r="Q8" s="4"/>
       <c r="R8" s="4"/>
-      <c r="S8" s="4"/>
+      <c r="S8" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="T8" s="4"/>
       <c r="U8" s="4"/>
       <c r="V8" s="4"/>
@@ -828,7 +836,9 @@
       <c r="Q9" s="5"/>
       <c r="R9" s="4"/>
       <c r="S9" s="4"/>
-      <c r="T9" s="4"/>
+      <c r="T9" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="U9" s="4"/>
       <c r="V9" s="4"/>
       <c r="W9" s="4"/>
@@ -869,7 +879,9 @@
       <c r="S10" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T10" s="4"/>
+      <c r="T10" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="U10" s="4"/>
       <c r="V10" s="4"/>
       <c r="W10" s="4"/>
@@ -908,7 +920,9 @@
       <c r="S11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="T11" s="5"/>
+      <c r="T11" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="U11" s="4"/>
       <c r="V11" s="4"/>
       <c r="W11" s="4"/>
@@ -941,7 +955,7 @@
       <c r="Q12" s="4"/>
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
-      <c r="T12" s="5"/>
+      <c r="T12" s="6"/>
       <c r="U12" s="5"/>
       <c r="V12" s="4"/>
       <c r="W12" s="4"/>

</xml_diff>

<commit_message>
Final commit: all modeling completed, all project files run and included (folder structure not fully organized due to time constraints :(  )
</commit_message>
<xml_diff>
--- a/documentation/working_schedule.xlsx
+++ b/documentation/working_schedule.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ebrarsudedogan/PycharmProjects/Mining-Retail-Behavior-in-Istanbul-Malls-Using-Consumer-Sentiment-Indices/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{445F99A3-2690-E44D-8CD1-6D083A24CBFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E0CEEBD-E84A-394C-95BD-ACC71AC69B99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="14280" xr2:uid="{900F4403-C22E-0342-A1F2-D386E10D2AC7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="26">
   <si>
     <t>Veri Toplama</t>
   </si>
@@ -551,7 +551,7 @@
   <dimension ref="B3:X18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="T6" sqref="T6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -956,8 +956,10 @@
       <c r="R12" s="4"/>
       <c r="S12" s="4"/>
       <c r="T12" s="6"/>
-      <c r="U12" s="5"/>
-      <c r="V12" s="4"/>
+      <c r="U12" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="V12" s="6"/>
       <c r="W12" s="4"/>
       <c r="X12" s="4"/>
     </row>
@@ -989,8 +991,10 @@
       <c r="R13" s="4"/>
       <c r="S13" s="4"/>
       <c r="T13" s="4"/>
-      <c r="U13" s="5"/>
-      <c r="V13" s="5"/>
+      <c r="U13" s="6"/>
+      <c r="V13" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="W13" s="4"/>
       <c r="X13" s="4"/>
     </row>
@@ -1020,7 +1024,9 @@
       <c r="R14" s="4"/>
       <c r="S14" s="4"/>
       <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
+      <c r="U14" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="V14" s="5"/>
       <c r="W14" s="4"/>
       <c r="X14" s="4"/>
@@ -1054,7 +1060,9 @@
       <c r="S15" s="4"/>
       <c r="T15" s="4"/>
       <c r="U15" s="4"/>
-      <c r="V15" s="5"/>
+      <c r="V15" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="W15" s="5"/>
       <c r="X15" s="4"/>
     </row>
@@ -1086,10 +1094,16 @@
       <c r="R16" s="4"/>
       <c r="S16" s="4"/>
       <c r="T16" s="4"/>
-      <c r="U16" s="4"/>
+      <c r="U16" s="6" t="s">
+        <v>13</v>
+      </c>
       <c r="V16" s="4"/>
-      <c r="W16" s="5"/>
-      <c r="X16" s="5"/>
+      <c r="W16" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="X16" s="6" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B17" s="1"/>

</xml_diff>